<commit_message>
ændret i et excel ark Test
</commit_message>
<xml_diff>
--- a/Assets/Excel Budget/test.xlsx
+++ b/Assets/Excel Budget/test.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,86 +454,98 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="C4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="D4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="E4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="F4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="G4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="H4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="I4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="J4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="K4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="L4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="M4">
-        <v>17500</v>
+        <v>4560</v>
       </c>
       <c r="N4">
         <f>SUM(B4:M4)</f>
-        <v>210000</v>
+        <v>54720</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5">
-        <v>17500</v>
+        <f>SUM(B2:B4)</f>
+        <v>4560</v>
       </c>
       <c r="C5">
-        <v>17500</v>
+        <f t="shared" ref="C5:N5" si="0">SUM(C2:C4)</f>
+        <v>4560</v>
       </c>
       <c r="D5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="E5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="F5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="G5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="H5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="I5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="J5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="K5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="L5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="M5">
-        <v>17500</v>
+        <f t="shared" si="0"/>
+        <v>4560</v>
       </c>
       <c r="N5">
-        <f>SUM(B5:M5)</f>
-        <v>210000</v>
+        <f t="shared" si="0"/>
+        <v>54720</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -596,51 +608,51 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f ca="1">SUM(B12:B16)</f>
+        <f t="shared" ref="B14:M14" ca="1" si="1">SUM(B12:B16)</f>
         <v>2038</v>
       </c>
       <c r="C14">
-        <f ca="1">SUM(C12:C16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>10500</v>
       </c>
       <c r="D14">
-        <f ca="1">SUM(D12:D16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2038</v>
       </c>
       <c r="E14">
-        <f ca="1">SUM(E12:E16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f ca="1">SUM(F12:F16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>12538</v>
       </c>
       <c r="G14">
-        <f ca="1">SUM(G12:G16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f ca="1">SUM(H12:H16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2038</v>
       </c>
       <c r="I14">
-        <f ca="1">SUM(I12:I16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>10500</v>
       </c>
       <c r="J14">
-        <f ca="1">SUM(J12:J16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>2038</v>
       </c>
       <c r="K14">
-        <f ca="1">SUM(K12:K16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f ca="1">SUM(L12:L16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>12538</v>
       </c>
       <c r="M14">
-        <f ca="1">SUM(M12:M16)</f>
+        <f t="shared" ca="1" si="1"/>
         <v>0</v>
       </c>
       <c r="N14">

</xml_diff>

<commit_message>
ændringer fra i fredags + NYE OG LÆNGERE BEN TIL BORDET ;);););)
</commit_message>
<xml_diff>
--- a/Assets/Excel Budget/test.xlsx
+++ b/Assets/Excel Budget/test.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,56 +608,56 @@
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
-        <f t="shared" ref="B14:M14" ca="1" si="1">SUM(B12:B16)</f>
-        <v>2038</v>
+        <f>SUM(B12:B13)</f>
+        <v>23</v>
       </c>
       <c r="C14">
-        <f t="shared" ca="1" si="1"/>
-        <v>10500</v>
+        <f>SUM(C12:C13)</f>
+        <v>1500</v>
       </c>
       <c r="D14">
-        <f t="shared" ca="1" si="1"/>
-        <v>2038</v>
+        <f t="shared" ref="D14:N14" si="1">SUM(D12:D13)</f>
+        <v>23</v>
       </c>
       <c r="E14">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="1"/>
-        <v>12538</v>
+        <f t="shared" si="1"/>
+        <v>1523</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H14">
-        <f t="shared" ca="1" si="1"/>
-        <v>2038</v>
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="I14">
-        <f t="shared" ca="1" si="1"/>
-        <v>10500</v>
+        <f t="shared" si="1"/>
+        <v>1500</v>
       </c>
       <c r="J14">
-        <f t="shared" ca="1" si="1"/>
-        <v>2038</v>
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="K14">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" ca="1" si="1"/>
-        <v>12538</v>
+        <f t="shared" si="1"/>
+        <v>1523</v>
       </c>
       <c r="M14">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="N14">
-        <f ca="1">SUM(B14:M14)</f>
-        <v>54228</v>
+        <f t="shared" si="1"/>
+        <v>6138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pengeposer og alt det andet lækkert
</commit_message>
<xml_diff>
--- a/Assets/Excel Budget/test.xlsx
+++ b/Assets/Excel Budget/test.xlsx
@@ -396,7 +396,7 @@
   <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -454,98 +454,98 @@
         <v>16</v>
       </c>
       <c r="B4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="C4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="D4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="E4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="F4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="G4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="H4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="I4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="J4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="K4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="L4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="M4">
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="N4">
         <f>SUM(B4:M4)</f>
-        <v>54720</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5">
         <f>SUM(B2:B4)</f>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="C5">
         <f t="shared" ref="C5:N5" si="0">SUM(C2:C4)</f>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="D5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="F5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="G5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="H5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="I5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="J5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="K5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="M5">
         <f t="shared" si="0"/>
-        <v>4560</v>
+        <v>1000</v>
       </c>
       <c r="N5">
         <f t="shared" si="0"/>
-        <v>54720</v>
+        <v>12000</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
@@ -563,26 +563,26 @@
         <v>17</v>
       </c>
       <c r="B12">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="D12">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="F12">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="H12">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="J12">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="L12">
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="N12">
         <f>SUM(B12:M12)</f>
-        <v>138</v>
+        <v>720</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -590,34 +590,34 @@
         <v>18</v>
       </c>
       <c r="C13">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="F13">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="I13">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="L13">
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="N13">
         <f>SUM(B13:M13)</f>
-        <v>6000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <f>SUM(B12:B13)</f>
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="C14">
         <f>SUM(C12:C13)</f>
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="D14">
         <f t="shared" ref="D14:N14" si="1">SUM(D12:D13)</f>
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="E14">
         <f t="shared" si="1"/>
@@ -625,7 +625,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="1"/>
-        <v>1523</v>
+        <v>1320</v>
       </c>
       <c r="G14">
         <f t="shared" si="1"/>
@@ -633,15 +633,15 @@
       </c>
       <c r="H14">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="I14">
         <f t="shared" si="1"/>
-        <v>1500</v>
+        <v>1200</v>
       </c>
       <c r="J14">
         <f t="shared" si="1"/>
-        <v>23</v>
+        <v>120</v>
       </c>
       <c r="K14">
         <f t="shared" si="1"/>
@@ -649,7 +649,7 @@
       </c>
       <c r="L14">
         <f t="shared" si="1"/>
-        <v>1523</v>
+        <v>1320</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
@@ -657,7 +657,7 @@
       </c>
       <c r="N14">
         <f t="shared" si="1"/>
-        <v>6138</v>
+        <v>5520</v>
       </c>
     </row>
   </sheetData>

</xml_diff>